<commit_message>
- Corrigé les noms des paroisses dans les fichiers de la région 9.
git-svn-id: https://svn.opac.ch/svn/cr/branches/vs2010.1@20011 787ff09c-d2b5-7842-b444-8dd0a418631d
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/App.Aider/Samples/EERV Région 9/9010/id.xlsx
+++ b/Epsitec.Cresus/App.Aider/Samples/EERV Région 9/9010/id.xlsx
@@ -39,22 +39,22 @@
     <t>Stockage</t>
   </si>
   <si>
-    <t>Pully-Paudex</t>
-  </si>
-  <si>
-    <t>Belmont-Lutry</t>
-  </si>
-  <si>
     <t>Saint-Saphorin</t>
   </si>
   <si>
-    <t>Savigny-Forel</t>
-  </si>
-  <si>
     <t>Villette</t>
   </si>
   <si>
     <t>Région 9 Lavaux</t>
+  </si>
+  <si>
+    <t>Pully – Paudex</t>
+  </si>
+  <si>
+    <t>Belmont – Lutry</t>
+  </si>
+  <si>
+    <t>Savigny – Forel</t>
   </si>
 </sst>
 </file>
@@ -460,7 +460,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D16:D17"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -499,7 +499,7 @@
         <v>9000</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F2" s="7">
         <v>1</v>
@@ -519,7 +519,7 @@
         <v>9000</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F3" s="7">
         <v>1</v>
@@ -539,7 +539,7 @@
         <v>9000</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F4" s="7">
         <v>1</v>
@@ -559,7 +559,7 @@
         <v>9000</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F5" s="7">
         <v>1</v>
@@ -579,7 +579,7 @@
         <v>9000</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F6" s="7">
         <v>1</v>
@@ -599,7 +599,7 @@
         <v>9000</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F7" s="7">
         <v>1</v>

</xml_diff>